<commit_message>
Communication links WC1-3 hinzugefügt
</commit_message>
<xml_diff>
--- a/Threagile_fullrun/risks.xlsx
+++ b/Threagile_fullrun/risks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="222">
   <si>
     <t>Severity</t>
   </si>
@@ -205,6 +205,30 @@
     <t>Unlikely</t>
   </si>
   <si>
+    <t>Spoofing</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>CWE-287</t>
+  </si>
+  <si>
+    <t>Missing Identity Store</t>
+  </si>
+  <si>
+    <t>Missing Identity Store in the threat model (referencing asset S3 as an example)</t>
+  </si>
+  <si>
+    <t>Identity Store</t>
+  </si>
+  <si>
+    <t>Include an identity store in the model if the application has a login.</t>
+  </si>
+  <si>
+    <t>missing-identity-store@S3</t>
+  </si>
+  <si>
     <t>Elevation of Privilege</t>
   </si>
   <si>
@@ -247,9 +271,6 @@
     <t>Information Disclosure</t>
   </si>
   <si>
-    <t>Architecture</t>
-  </si>
-  <si>
     <t>CWE-522</t>
   </si>
   <si>
@@ -379,6 +400,42 @@
     <t>unchecked-deployment@S5</t>
   </si>
   <si>
+    <t>Unnecessary Communication Link</t>
+  </si>
+  <si>
+    <t>WC1-to-S3</t>
+  </si>
+  <si>
+    <t>Unnecessary Communication Link titled WC1-to-S3 at technical asset WC1</t>
+  </si>
+  <si>
+    <t>Attack Surface Reduction</t>
+  </si>
+  <si>
+    <t>Try to avoid using technical communication links that do not send or receive anything.</t>
+  </si>
+  <si>
+    <t>unnecessary-communication-link@WC1&gt;wc1-to-s3@WC1</t>
+  </si>
+  <si>
+    <t>WC2-to-S3</t>
+  </si>
+  <si>
+    <t>Unnecessary Communication Link titled WC2-to-S3 at technical asset WC2</t>
+  </si>
+  <si>
+    <t>unnecessary-communication-link@WC2&gt;wc2-to-s3@WC2</t>
+  </si>
+  <si>
+    <t>WC3-to-S3</t>
+  </si>
+  <si>
+    <t>Unnecessary Communication Link titled WC3-to-S3 at technical asset WC3</t>
+  </si>
+  <si>
+    <t>unnecessary-communication-link@WC3&gt;wc3-to-s3@WC3</t>
+  </si>
+  <si>
     <t>Unnecessary Technical Asset</t>
   </si>
   <si>
@@ -388,9 +445,6 @@
     <t>Unnecessary Technical Asset named C2</t>
   </si>
   <si>
-    <t>Attack Surface Reduction</t>
-  </si>
-  <si>
     <t>Try to avoid using technical assets that do not process or store anything.</t>
   </si>
   <si>
@@ -517,12 +571,6 @@
     <t>unnecessary-technical-asset@S2</t>
   </si>
   <si>
-    <t>Unnecessary Technical Asset named S3</t>
-  </si>
-  <si>
-    <t>unnecessary-technical-asset@S3</t>
-  </si>
-  <si>
     <t>Unnecessary Technical Asset named S4</t>
   </si>
   <si>
@@ -553,31 +601,37 @@
     <t>unnecessary-technical-asset@T2</t>
   </si>
   <si>
-    <t>Unnecessary Technical Asset named WC1</t>
-  </si>
-  <si>
-    <t>unnecessary-technical-asset@WC1</t>
-  </si>
-  <si>
-    <t>Unnecessary Technical Asset named WC2</t>
-  </si>
-  <si>
-    <t>unnecessary-technical-asset@WC2</t>
-  </si>
-  <si>
-    <t>Unnecessary Technical Asset named WC3</t>
-  </si>
-  <si>
-    <t>unnecessary-technical-asset@WC3</t>
+    <t>Wrong Communication Link Content</t>
+  </si>
+  <si>
+    <t>Wrong Communication Link Content (data assets sent/received not matching the communication link's readonly flag) at WC1 regarding communication link WC1-to-S3</t>
+  </si>
+  <si>
+    <t>Model Consistency</t>
+  </si>
+  <si>
+    <t>Try to model the correct readonly flag and/or data sent/received of communication links. Also try to use  communication link types matching the target technology/machine types.</t>
+  </si>
+  <si>
+    <t>wrong-communication-link-content@WC1@WC1&gt;wc1-to-s3</t>
+  </si>
+  <si>
+    <t>Wrong Communication Link Content (data assets sent/received not matching the communication link's readonly flag) at WC2 regarding communication link WC2-to-S3</t>
+  </si>
+  <si>
+    <t>wrong-communication-link-content@WC2@WC2&gt;wc2-to-s3</t>
+  </si>
+  <si>
+    <t>Wrong Communication Link Content (data assets sent/received not matching the communication link's readonly flag) at WC3 regarding communication link WC3-to-S3</t>
+  </si>
+  <si>
+    <t>wrong-communication-link-content@WC3@WC3&gt;wc3-to-s3</t>
   </si>
   <si>
     <t>Wrong Trust Boundary Content</t>
   </si>
   <si>
     <t>Wrong Trust Boundary Content (non-container asset inside container trust boundary) at DC2</t>
-  </si>
-  <si>
-    <t>Model Consistency</t>
   </si>
   <si>
     <t>Try to model the correct types of trust boundaries and data assets.</t>
@@ -1466,7 +1520,7 @@
         <v>28</v>
       </c>
       <c r="J6" s="18">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K6" s="19" t="s">
         <v>45</v>
@@ -1667,22 +1721,22 @@
         <v>63</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J10" s="18">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="K10" s="19" t="s">
         <v>67</v>
@@ -1718,19 +1772,19 @@
         <v>22</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>54</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>28</v>
@@ -1739,19 +1793,19 @@
         <v>52</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="N11" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O11" s="20" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="P11" s="10" t="s">
         <v>34</v>
@@ -1762,50 +1816,50 @@
       <c r="T11" s="16"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="10" t="s">
+      <c r="A12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="I12" s="9" t="s">
+      <c r="F12" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J12" s="18">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="N12" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="P12" s="10" t="s">
         <v>34</v>
@@ -1816,50 +1870,50 @@
       <c r="T12" s="16"/>
     </row>
     <row r="13">
-      <c r="A13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="8" t="s">
+      <c r="A13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="18">
+        <v>100</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="L13" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="M13" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="18">
-        <v>52</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="L13" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="M13" s="22" t="s">
-        <v>82</v>
-      </c>
       <c r="N13" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O13" s="20" t="s">
         <v>83</v>
-      </c>
-      <c r="O13" s="20" t="s">
-        <v>84</v>
       </c>
       <c r="P13" s="10" t="s">
         <v>34</v>
@@ -1877,22 +1931,22 @@
         <v>62</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>87</v>
-      </c>
       <c r="H14" s="7" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>28</v>
@@ -1901,16 +1955,16 @@
         <v>52</v>
       </c>
       <c r="K14" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="L14" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="L14" s="22" t="s">
+      <c r="M14" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="M14" s="22" t="s">
+      <c r="N14" s="22" t="s">
         <v>90</v>
-      </c>
-      <c r="N14" s="22" t="s">
-        <v>32</v>
       </c>
       <c r="O14" s="20" t="s">
         <v>91</v>
@@ -1931,22 +1985,22 @@
         <v>62</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>54</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>28</v>
@@ -1955,19 +2009,19 @@
         <v>52</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="L15" s="22" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="M15" s="22" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="N15" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O15" s="20" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="P15" s="10" t="s">
         <v>34</v>
@@ -1985,43 +2039,43 @@
         <v>62</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>54</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J16" s="18">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="K16" s="19" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="L16" s="22" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="M16" s="22" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="N16" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O16" s="20" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="P16" s="10" t="s">
         <v>34</v>
@@ -2042,40 +2096,40 @@
         <v>22</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>54</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="H17" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="18">
+        <v>34</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="L17" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="M17" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17" s="18">
-        <v>40</v>
-      </c>
-      <c r="K17" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="L17" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="M17" s="22" t="s">
-        <v>90</v>
-      </c>
       <c r="N17" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O17" s="20" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="P17" s="10" t="s">
         <v>34</v>
@@ -2096,19 +2150,19 @@
         <v>22</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>54</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="I18" s="7" t="s">
         <v>28</v>
@@ -2117,19 +2171,19 @@
         <v>40</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="L18" s="22" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="N18" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O18" s="20" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="P18" s="10" t="s">
         <v>34</v>
@@ -2150,40 +2204,40 @@
         <v>22</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>54</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="I19" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J19" s="18">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L19" s="22" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="M19" s="22" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="N19" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O19" s="20" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="P19" s="10" t="s">
         <v>34</v>
@@ -2204,40 +2258,40 @@
         <v>22</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>54</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J20" s="18">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="L20" s="22" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="M20" s="22" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="N20" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O20" s="20" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="P20" s="10" t="s">
         <v>34</v>
@@ -2258,19 +2312,19 @@
         <v>22</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>54</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I21" s="7" t="s">
         <v>28</v>
@@ -2279,19 +2333,19 @@
         <v>33</v>
       </c>
       <c r="K21" s="19" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="L21" s="22" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="M21" s="22" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="N21" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O21" s="20" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="P21" s="10" t="s">
         <v>34</v>
@@ -2302,44 +2356,44 @@
       <c r="T21" s="16"/>
     </row>
     <row r="22">
-      <c r="A22" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" s="10" t="s">
+      <c r="A22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="I22" s="9" t="s">
+      <c r="F22" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I22" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J22" s="18">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="K22" s="19" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="M22" s="22" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="N22" s="22" t="s">
         <v>32</v>
@@ -2366,10 +2420,10 @@
         <v>53</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>116</v>
@@ -2378,7 +2432,7 @@
         <v>117</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="I23" s="9" t="s">
         <v>28</v>
@@ -2387,19 +2441,19 @@
         <v>14</v>
       </c>
       <c r="K23" s="19" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L23" s="22" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="M23" s="22" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="N23" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O23" s="20" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="P23" s="10" t="s">
         <v>34</v>
@@ -2420,40 +2474,40 @@
         <v>53</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I24" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J24" s="18">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="K24" s="19" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L24" s="22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="M24" s="22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="N24" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O24" s="20" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="P24" s="10" t="s">
         <v>34</v>
@@ -2474,40 +2528,40 @@
         <v>53</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>28</v>
+        <v>129</v>
       </c>
       <c r="J25" s="18">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="K25" s="19" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L25" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M25" s="22" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="N25" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O25" s="20" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="P25" s="10" t="s">
         <v>34</v>
@@ -2528,40 +2582,40 @@
         <v>53</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>28</v>
+        <v>134</v>
       </c>
       <c r="J26" s="18">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="K26" s="19" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="L26" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M26" s="22" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="N26" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O26" s="20" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="P26" s="10" t="s">
         <v>34</v>
@@ -2582,40 +2636,40 @@
         <v>53</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="H27" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J27" s="18">
+        <v>33</v>
+      </c>
+      <c r="K27" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="L27" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J27" s="18">
-        <v>3</v>
-      </c>
-      <c r="K27" s="19" t="s">
+      <c r="M27" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="L27" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="M27" s="22" t="s">
-        <v>125</v>
-      </c>
       <c r="N27" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O27" s="20" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="P27" s="10" t="s">
         <v>34</v>
@@ -2636,40 +2690,40 @@
         <v>53</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J28" s="18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="L28" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M28" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N28" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O28" s="20" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="P28" s="10" t="s">
         <v>34</v>
@@ -2690,40 +2744,40 @@
         <v>53</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="I29" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J29" s="18">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="K29" s="19" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="L29" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M29" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N29" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O29" s="20" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="P29" s="10" t="s">
         <v>34</v>
@@ -2744,40 +2798,40 @@
         <v>53</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
       <c r="I30" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J30" s="18">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="L30" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M30" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N30" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O30" s="20" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="P30" s="10" t="s">
         <v>34</v>
@@ -2798,40 +2852,40 @@
         <v>53</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H31" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J31" s="18">
+        <v>3</v>
+      </c>
+      <c r="K31" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="L31" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="M31" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J31" s="18">
-        <v>7</v>
-      </c>
-      <c r="K31" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="L31" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="M31" s="22" t="s">
-        <v>125</v>
-      </c>
       <c r="N31" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O31" s="20" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="P31" s="10" t="s">
         <v>34</v>
@@ -2852,40 +2906,40 @@
         <v>53</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="I32" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J32" s="18">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="K32" s="19" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="L32" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M32" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N32" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O32" s="20" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P32" s="10" t="s">
         <v>34</v>
@@ -2906,40 +2960,40 @@
         <v>53</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="I33" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J33" s="18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K33" s="19" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="L33" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M33" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N33" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O33" s="20" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="P33" s="10" t="s">
         <v>34</v>
@@ -2960,40 +3014,40 @@
         <v>53</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="I34" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J34" s="18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="L34" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M34" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N34" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O34" s="20" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="P34" s="10" t="s">
         <v>34</v>
@@ -3014,40 +3068,40 @@
         <v>53</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="I35" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J35" s="18">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K35" s="19" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="L35" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M35" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N35" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O35" s="20" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="P35" s="10" t="s">
         <v>34</v>
@@ -3068,40 +3122,40 @@
         <v>53</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="I36" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J36" s="18">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="K36" s="19" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="L36" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M36" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N36" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O36" s="20" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="P36" s="10" t="s">
         <v>34</v>
@@ -3122,40 +3176,40 @@
         <v>53</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>27</v>
+        <v>166</v>
       </c>
       <c r="I37" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J37" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K37" s="19" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="L37" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M37" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N37" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O37" s="20" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="P37" s="10" t="s">
         <v>34</v>
@@ -3176,19 +3230,19 @@
         <v>53</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>35</v>
+        <v>169</v>
       </c>
       <c r="I38" s="9" t="s">
         <v>28</v>
@@ -3197,19 +3251,19 @@
         <v>1</v>
       </c>
       <c r="K38" s="19" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="L38" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M38" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N38" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O38" s="20" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="P38" s="10" t="s">
         <v>34</v>
@@ -3230,40 +3284,40 @@
         <v>53</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="I39" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J39" s="18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K39" s="19" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="L39" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M39" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N39" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O39" s="20" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="P39" s="10" t="s">
         <v>34</v>
@@ -3284,40 +3338,40 @@
         <v>53</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>38</v>
+        <v>175</v>
       </c>
       <c r="I40" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J40" s="18">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="K40" s="19" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="L40" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M40" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N40" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O40" s="20" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="P40" s="10" t="s">
         <v>34</v>
@@ -3338,19 +3392,19 @@
         <v>53</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="I41" s="9" t="s">
         <v>28</v>
@@ -3359,19 +3413,19 @@
         <v>5</v>
       </c>
       <c r="K41" s="19" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="L41" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M41" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N41" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O41" s="20" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="P41" s="10" t="s">
         <v>34</v>
@@ -3392,40 +3446,40 @@
         <v>53</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>111</v>
+        <v>35</v>
       </c>
       <c r="I42" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J42" s="18">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="K42" s="19" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="L42" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M42" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N42" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O42" s="20" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="P42" s="10" t="s">
         <v>34</v>
@@ -3446,40 +3500,40 @@
         <v>53</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>57</v>
+        <v>182</v>
       </c>
       <c r="I43" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J43" s="18">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="K43" s="19" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="L43" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M43" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N43" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O43" s="20" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="P43" s="10" t="s">
         <v>34</v>
@@ -3500,40 +3554,40 @@
         <v>53</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="I44" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J44" s="18">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="K44" s="19" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="L44" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M44" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N44" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O44" s="20" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="P44" s="10" t="s">
         <v>34</v>
@@ -3554,40 +3608,40 @@
         <v>53</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="I45" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J45" s="18">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="K45" s="19" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="L45" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M45" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N45" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O45" s="20" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="P45" s="10" t="s">
         <v>34</v>
@@ -3608,40 +3662,40 @@
         <v>53</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="I46" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J46" s="18">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="K46" s="19" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="L46" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M46" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N46" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O46" s="20" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="P46" s="10" t="s">
         <v>34</v>
@@ -3662,40 +3716,40 @@
         <v>53</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="I47" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J47" s="18">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="K47" s="19" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="L47" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M47" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N47" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O47" s="20" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="P47" s="10" t="s">
         <v>34</v>
@@ -3716,40 +3770,40 @@
         <v>53</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="H48" s="9" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="I48" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J48" s="18">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="K48" s="19" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="L48" s="22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M48" s="22" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N48" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O48" s="20" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="P48" s="10" t="s">
         <v>34</v>
@@ -3770,40 +3824,40 @@
         <v>53</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>28</v>
+        <v>129</v>
       </c>
       <c r="J49" s="18">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="K49" s="19" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="L49" s="22" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="M49" s="22" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="N49" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O49" s="20" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="P49" s="10" t="s">
         <v>34</v>
@@ -3824,40 +3878,40 @@
         <v>53</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="H50" s="9" t="s">
-        <v>131</v>
+        <v>47</v>
       </c>
       <c r="I50" s="9" t="s">
-        <v>28</v>
+        <v>134</v>
       </c>
       <c r="J50" s="18">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="K50" s="19" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="L50" s="22" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="M50" s="22" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="N50" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O50" s="20" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="P50" s="10" t="s">
         <v>34</v>
@@ -3878,40 +3932,40 @@
         <v>53</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="H51" s="9" t="s">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="I51" s="9" t="s">
-        <v>28</v>
+        <v>137</v>
       </c>
       <c r="J51" s="18">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="K51" s="19" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="L51" s="22" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="M51" s="22" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="N51" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O51" s="20" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="P51" s="10" t="s">
         <v>34</v>
@@ -3932,40 +3986,40 @@
         <v>53</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="H52" s="9" t="s">
-        <v>154</v>
+        <v>104</v>
       </c>
       <c r="I52" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J52" s="18">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="K52" s="19" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="L52" s="22" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="M52" s="22" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="N52" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O52" s="20" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="P52" s="10" t="s">
         <v>34</v>
@@ -3986,40 +4040,40 @@
         <v>53</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="H53" s="9" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="I53" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J53" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K53" s="19" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="L53" s="22" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="M53" s="22" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="N53" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O53" s="20" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="P53" s="10" t="s">
         <v>34</v>
@@ -4040,40 +4094,40 @@
         <v>53</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="H54" s="9" t="s">
-        <v>35</v>
+        <v>107</v>
       </c>
       <c r="I54" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J54" s="18">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="K54" s="19" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="L54" s="22" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="M54" s="22" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="N54" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O54" s="20" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="P54" s="10" t="s">
         <v>34</v>
@@ -4094,40 +4148,40 @@
         <v>53</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="H55" s="9" t="s">
-        <v>66</v>
+        <v>172</v>
       </c>
       <c r="I55" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J55" s="18">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="K55" s="19" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="L55" s="22" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="M55" s="22" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="N55" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O55" s="20" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="P55" s="10" t="s">
         <v>34</v>
@@ -4148,40 +4202,40 @@
         <v>53</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>71</v>
+        <v>175</v>
       </c>
       <c r="I56" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J56" s="18">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="K56" s="19" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="L56" s="22" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="M56" s="22" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="N56" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O56" s="20" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="P56" s="10" t="s">
         <v>34</v>
@@ -4190,6 +4244,168 @@
       <c r="R56" s="17"/>
       <c r="S56" s="17"/>
       <c r="T56" s="16"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I57" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J57" s="18">
+        <v>1</v>
+      </c>
+      <c r="K57" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="L57" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="M57" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="N57" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O57" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="P57" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q57" s="19"/>
+      <c r="R57" s="17"/>
+      <c r="S57" s="17"/>
+      <c r="T57" s="16"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I58" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J58" s="18">
+        <v>52</v>
+      </c>
+      <c r="K58" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="L58" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="M58" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="N58" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O58" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="P58" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q58" s="19"/>
+      <c r="R58" s="17"/>
+      <c r="S58" s="17"/>
+      <c r="T58" s="16"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I59" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J59" s="18">
+        <v>52</v>
+      </c>
+      <c r="K59" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="L59" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="M59" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="N59" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O59" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="P59" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q59" s="19"/>
+      <c r="R59" s="17"/>
+      <c r="S59" s="17"/>
+      <c r="T59" s="16"/>
     </row>
   </sheetData>
   <pageSetup orientation="landscape" paperSize="9"/>

</xml_diff>